<commit_message>
Sync data files - 2025-07-22 13:05:28 (       1 files updated)
</commit_message>
<xml_diff>
--- a/Data/Rentals/Sidra_rentals.xlsx
+++ b/Data/Rentals/Sidra_rentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levan/Documents/MegaValuationer/Data/Rentals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E3E79E-8225-DE4B-9A59-67EB6EFA0ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19010D8-3DEF-7D4D-9662-D7864ED4316B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{BFAD7A34-5F38-5B44-9431-430E2A8DC87D}"/>
+    <workbookView xWindow="0" yWindow="9940" windowWidth="29400" windowHeight="9180" xr2:uid="{BFAD7A34-5F38-5B44-9431-430E2A8DC87D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4023,9 +4023,6 @@
     <t> 12 Jul 2025 / 11 Jul 2026</t>
   </si>
   <si>
-    <t>Sub Community / Building</t>
-  </si>
-  <si>
     <t>Evidence Date</t>
   </si>
   <si>
@@ -4066,6 +4063,9 @@
   </si>
   <si>
     <t>Rent Recurrence</t>
+  </si>
+  <si>
+    <t>Sub Community/Building</t>
   </si>
 </sst>
 </file>
@@ -4440,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8D60B8-FE63-CF4C-B4E0-7888309BA827}">
   <dimension ref="A1:O1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4465,49 +4465,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B1" t="s">
         <v>1328</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1329</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1330</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F1" t="s">
         <v>1331</v>
       </c>
-      <c r="E1" t="s">
-        <v>1327</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1332</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1333</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1334</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1335</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1336</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>1337</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>1338</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>1339</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>1340</v>
-      </c>
-      <c r="O1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>